<commit_message>
Update filtering, sorting pagnigation product
</commit_message>
<xml_diff>
--- a/server/uploads/data.xlsx
+++ b/server/uploads/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD8998A-5D8A-4538-88CA-A080865C30D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609CD965-ED21-499C-9FF6-4F44575B730B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,12 +33,6 @@
     <t>price</t>
   </si>
   <si>
-    <t>Iphone 15</t>
-  </si>
-  <si>
-    <t>samsung</t>
-  </si>
-  <si>
     <t>brand</t>
   </si>
   <si>
@@ -55,6 +49,12 @@
   </si>
   <si>
     <t>description 2</t>
+  </si>
+  <si>
+    <t>Iphone 17</t>
+  </si>
+  <si>
+    <t>samsung 10</t>
   </si>
 </sst>
 </file>
@@ -381,51 +381,54 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>